<commit_message>
Updated sentiment dataset info
</commit_message>
<xml_diff>
--- a/data_exploration/acl/tables/sentiment_text_types.xlsx
+++ b/data_exploration/acl/tables/sentiment_text_types.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="122">
   <si>
     <t>Language</t>
   </si>
@@ -288,13 +288,115 @@
   </si>
   <si>
     <t>https://github.com/kcortis/malta-budget-social-opinion</t>
+  </si>
+  <si>
+    <t>Social media, Reviews</t>
+  </si>
+  <si>
+    <t>https://www.kaggle.com/ilhamfp31/dataset-prosa</t>
+  </si>
+  <si>
+    <t>https://arxiv.org/ftp/arxiv/papers/2009/2009.05720.pdf</t>
+  </si>
+  <si>
+    <t>Human annotated</t>
+  </si>
+  <si>
+    <t>https://github.com/irwanafandi24/Sentiment-Analysis-on-Twitter</t>
+  </si>
+  <si>
+    <t>Used in train</t>
+  </si>
+  <si>
+    <t>Used in validation</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/drive/folders/1xclbjHHK58zk2X6iqbvMPS2rcy9y9E0X</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1flr5ew6thRFw4emMx5hWlAS3gUYBp8bI/view</t>
+  </si>
+  <si>
+    <t>Feedback</t>
+  </si>
+  <si>
+    <t>Education</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>VSFC (Vietnamese Students’ Feedback Corpus)</t>
+  </si>
+  <si>
+    <t>VLSP 2016</t>
+  </si>
+  <si>
+    <t> NSMC (Naver Sentiment Movie Corpus)</t>
+  </si>
+  <si>
+    <t>KOSAC (KOrean Sentiment Analysis Corpus)</t>
+  </si>
+  <si>
+    <t>https://ieeexplore.ieee.org/abstract/document/9068897</t>
+  </si>
+  <si>
+    <t>https://github.com/adelabdelli/DzSentiA</t>
+  </si>
+  <si>
+    <t>https://github.com/kinmokusu/oea_algd</t>
+  </si>
+  <si>
+    <t>https://www.researchgate.net/publication/330702611_Construction_et_exploitation_d'un_corpus_multilingue_algerien_pour_l'analyse_des_opinions_et_des_emotions</t>
+  </si>
+  <si>
+    <t>https://www.researchgate.net/profile/Mhamed_Mataoui2/post/Any_available_algerian-dialect_tweets_dataset/attachment/59d6480079197b80779a2c03/AS%3A464939287617536%401487861572080/download/Dataset.rar</t>
+  </si>
+  <si>
+    <t>https://pdfs.semanticscholar.org/ac24/2bd92476bf4a8cce2808c2100a29da198a8e.pdf</t>
+  </si>
+  <si>
+    <t>https://github.com/iamaziz/ar-embeddings/tree/master/datasets</t>
+  </si>
+  <si>
+    <t>LABR (Large Arabic Book Reviews)</t>
+  </si>
+  <si>
+    <t>ASTD (Arabic Sentiment Tweets Dataset)</t>
+  </si>
+  <si>
+    <t>https://78462f86-a-fa7ed8f8-s-sites.googlegroups.com/a/mohamedaly.info/www/files/nabil2015astd.pdf?attachauth=ANoY7cqsaR1WwuodBUxRJ5FQWDOn4ddfdFmMg70fl42PsRjnLB0NKpWZ1wxDzuhqB3S3rkNI6a9SUIzHuIff4-3c6wT3y_pzBEKwySpcVqtxefRfp7DReThgBLHsVlhBPeNxuUeZMmYt6oW9IxxYeEGwKwa-E5rTLO0h88FB3GpsbQ-nN4Z-Guc6Ngh7dsE_8LRDwZaY_hFokDQZk5hM0bUZtnnu-nf6pQ%3D%3D&amp;attredirects=0</t>
+  </si>
+  <si>
+    <t>https://www.researchgate.net/publication/261427893_Arabic_sentiment_analysis_Lexicon-based_and_corpus-based</t>
+  </si>
+  <si>
+    <t>ArTwitter</t>
+  </si>
+  <si>
+    <t>https://sites.google.com/view/germeval2017-absa/data</t>
+  </si>
+  <si>
+    <t>Germeval 2017</t>
+  </si>
+  <si>
+    <t>Malta Budget 2018</t>
+  </si>
+  <si>
+    <t>https://www.inf.uni-hamburg.de/en/inst/ab/lt/publications/2017-wojatzkietal-germeval2017-workshop.pdf</t>
+  </si>
+  <si>
+    <t>Social media, Microblogs, Q&amp;A</t>
+  </si>
+  <si>
+    <t>Trains</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -318,8 +420,62 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -332,10 +488,89 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="8">
     <border>
       <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
       <right/>
       <top/>
       <bottom/>
@@ -346,14 +581,51 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -635,546 +907,972 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E40"/>
+  <dimension ref="A1:I49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" customWidth="1"/>
-    <col min="2" max="2" width="23.5703125" customWidth="1"/>
-    <col min="3" max="3" width="22.7109375" customWidth="1"/>
-    <col min="4" max="4" width="64.5703125" customWidth="1"/>
-    <col min="5" max="5" width="18.5703125" customWidth="1"/>
+    <col min="1" max="2" width="16.5703125" customWidth="1"/>
+    <col min="3" max="3" width="23.5703125" customWidth="1"/>
+    <col min="4" max="4" width="22.7109375" customWidth="1"/>
+    <col min="5" max="7" width="18" customWidth="1"/>
+    <col min="8" max="8" width="64.5703125" customWidth="1"/>
+    <col min="9" max="9" width="18.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>1</v>
+        <v>99</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>10</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="H2" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>117</v>
+      </c>
+      <c r="C3" t="s">
+        <v>120</v>
+      </c>
+      <c r="D3" t="s">
+        <v>121</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>12</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C4" t="s">
         <v>8</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D4" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="I4" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="5" spans="1:9" s="6" customFormat="1" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" s="30"/>
+      <c r="C5" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D5" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E5" s="6">
+        <v>1</v>
+      </c>
+      <c r="F5" s="6">
+        <v>1</v>
+      </c>
+      <c r="G5" s="6">
+        <v>1</v>
+      </c>
+      <c r="I5" s="8" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="6" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>17</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C6" t="s">
         <v>8</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D6" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="I6" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:5" s="3" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" s="3" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" s="3" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="C7" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="3">
+        <v>1</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" s="3" customFormat="1" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="D8" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="E8" s="3">
+        <v>0</v>
+      </c>
+      <c r="H8" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="E7" s="4"/>
-    </row>
-    <row r="8" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="I8" s="4"/>
+    </row>
+    <row r="9" spans="1:9" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C9" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D9" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="E9" s="15">
+        <v>1</v>
+      </c>
+      <c r="F9" s="15">
+        <v>1</v>
+      </c>
+      <c r="G9" s="15">
+        <v>1</v>
+      </c>
+      <c r="H9" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="I9" s="25" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:5" s="3" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+    <row r="10" spans="1:9" s="21" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="C10" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="D10" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="E10" s="21">
+        <v>0</v>
+      </c>
+      <c r="F10" s="21">
+        <v>1</v>
+      </c>
+      <c r="G10" s="21">
+        <v>1</v>
+      </c>
+      <c r="H10" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="E9" s="4"/>
-    </row>
-    <row r="10" spans="1:5" s="3" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+      <c r="I10" s="22"/>
+    </row>
+    <row r="11" spans="1:9" s="17" customFormat="1" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="C11" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="D11" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="E11" s="17">
+        <v>1</v>
+      </c>
+      <c r="F11" s="17">
+        <v>1</v>
+      </c>
+      <c r="G11" s="17">
+        <v>1</v>
+      </c>
+      <c r="H11" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="I11" s="18" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="12" spans="1:9" s="10" customFormat="1" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B12" s="31"/>
+      <c r="C12" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D12" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="E12" s="11">
+        <v>0</v>
+      </c>
+      <c r="F12" s="11">
+        <v>1</v>
+      </c>
+      <c r="G12" s="11">
+        <v>1</v>
+      </c>
+      <c r="H12" s="12" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="13" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>33</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B13" t="s">
+        <v>101</v>
+      </c>
+      <c r="C13" t="s">
         <v>9</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D13" t="s">
         <v>34</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E13" s="5">
+        <v>1</v>
+      </c>
+      <c r="F13" s="5">
+        <v>1</v>
+      </c>
+      <c r="G13" s="5">
+        <v>1</v>
+      </c>
+      <c r="H13" t="s">
         <v>7</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="I13" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:5" s="3" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
+    <row r="14" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>33</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B14" t="s">
+        <v>100</v>
+      </c>
+      <c r="C14" t="s">
+        <v>97</v>
+      </c>
+      <c r="D14" t="s">
+        <v>98</v>
+      </c>
+      <c r="E14" s="5">
+        <v>1</v>
+      </c>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" s="28" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="H15" s="29" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="16" spans="1:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
         <v>42</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C16" t="s">
         <v>21</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D16" t="s">
         <v>44</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="H16" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    <row r="17" spans="1:9" s="6" customFormat="1" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B17" s="30"/>
+      <c r="C17" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D17" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="E17" s="6">
+        <v>0</v>
+      </c>
+      <c r="F17" s="6">
+        <v>1</v>
+      </c>
+      <c r="G17" s="6">
+        <v>1</v>
+      </c>
+      <c r="H17" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="I17" s="8" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+    <row r="18" spans="1:9" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C18" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D18" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="E18" s="15">
+        <v>0</v>
+      </c>
+      <c r="F18" s="15">
+        <v>0</v>
+      </c>
+      <c r="G18" s="15">
+        <v>0</v>
+      </c>
+      <c r="H18" s="25" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:5" s="3" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
+    <row r="19" spans="1:9" s="21" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="C19" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="D19" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="E19" s="21">
+        <v>0</v>
+      </c>
+      <c r="F19" s="21">
+        <v>0</v>
+      </c>
+      <c r="G19" s="21">
+        <v>0</v>
+      </c>
+      <c r="H19" s="22" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    <row r="20" spans="1:9" s="21" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" s="32"/>
+      <c r="C20" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="D20" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="E20" s="21">
+        <v>1</v>
+      </c>
+      <c r="F20" s="21">
+        <v>1</v>
+      </c>
+      <c r="G20" s="21">
+        <v>1</v>
+      </c>
+      <c r="H20" s="22" t="s">
+        <v>89</v>
+      </c>
+      <c r="I20" s="22" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" s="17" customFormat="1" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="C21" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="D21" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="H21" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="I21" s="18"/>
+    </row>
+    <row r="22" spans="1:9" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C22" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D22" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E22" s="15">
+        <v>0</v>
+      </c>
+      <c r="F22" s="15">
+        <v>0</v>
+      </c>
+      <c r="G22" s="15">
+        <v>0</v>
+      </c>
+      <c r="H22" s="15" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="1:5" s="3" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
+    <row r="23" spans="1:9" s="17" customFormat="1" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B23" s="33"/>
+      <c r="C23" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="D23" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="E23" s="17">
+        <v>1</v>
+      </c>
+      <c r="F23" s="17">
+        <v>1</v>
+      </c>
+      <c r="G23" s="17">
+        <v>1</v>
+      </c>
+      <c r="H23" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="E19" s="5" t="s">
+      <c r="I23" s="19" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+    <row r="24" spans="1:9" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="38" t="s">
         <v>53</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C24" t="s">
         <v>9</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D24" t="s">
         <v>52</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="E24" s="5">
+        <v>1</v>
+      </c>
+      <c r="F24" s="26">
+        <v>1</v>
+      </c>
+      <c r="G24" s="26">
+        <v>1</v>
+      </c>
+      <c r="H24" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="I24" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+    <row r="25" spans="1:9" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B25" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="C25" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D25" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="D21" t="s">
+      <c r="E25" s="27">
+        <v>1</v>
+      </c>
+      <c r="F25" s="27">
+        <v>0</v>
+      </c>
+      <c r="G25" s="27">
+        <v>0</v>
+      </c>
+      <c r="H25" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="I25" s="25" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="22" spans="1:5" s="3" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
+    <row r="26" spans="1:9" s="17" customFormat="1" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B26" s="34" t="s">
+        <v>102</v>
+      </c>
+      <c r="C26" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="D26" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="D22" s="4" t="s">
+      <c r="E26" s="17">
+        <v>0</v>
+      </c>
+      <c r="F26" s="17">
+        <v>1</v>
+      </c>
+      <c r="G26" s="17">
+        <v>1</v>
+      </c>
+      <c r="H26" s="18" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+    <row r="27" spans="1:9" s="6" customFormat="1" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="B23" t="s">
+      <c r="C27" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C23" t="s">
+      <c r="D27" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="E27" s="7">
+        <v>0</v>
+      </c>
+      <c r="F27" s="7">
+        <v>1</v>
+      </c>
+      <c r="G27" s="7">
+        <v>1</v>
+      </c>
+      <c r="H27" s="8" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+    <row r="28" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="38" t="s">
         <v>66</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C28" t="s">
         <v>8</v>
       </c>
-      <c r="C24" t="s">
+      <c r="D28" t="s">
         <v>48</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="E28">
+        <v>1</v>
+      </c>
+      <c r="F28" s="26">
+        <v>1</v>
+      </c>
+      <c r="G28" s="26">
+        <v>1</v>
+      </c>
+      <c r="H28" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="E24" s="1" t="s">
+      <c r="I28" s="1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="25" spans="1:5" s="3" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
+    <row r="29" spans="1:9" s="3" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="38" t="s">
         <v>66</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="C29" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="D29" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D25" s="4" t="s">
+      <c r="E29" s="3">
+        <v>0</v>
+      </c>
+      <c r="F29" s="3">
+        <v>1</v>
+      </c>
+      <c r="G29" s="3">
+        <v>0</v>
+      </c>
+      <c r="H29" s="4" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="26" spans="1:5" s="3" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
+    <row r="30" spans="1:9" s="36" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="36" t="s">
         <v>66</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="C30" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="D30" s="36" t="s">
         <v>71</v>
       </c>
-      <c r="D26" s="4" t="s">
+      <c r="H30" s="37" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="27" spans="1:5" s="3" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
+    <row r="31" spans="1:9" s="3" customFormat="1" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="C31" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C27" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="D27" s="4" t="s">
+      <c r="H31" s="4" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+    <row r="32" spans="1:9" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="14" t="s">
         <v>73</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B32" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="C32" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C28" t="s">
+      <c r="D32" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="D28" s="1" t="s">
+      <c r="E32" s="15">
+        <v>0</v>
+      </c>
+      <c r="F32" s="15">
+        <v>0</v>
+      </c>
+      <c r="G32" s="15">
+        <v>0</v>
+      </c>
+      <c r="H32" s="25" t="s">
         <v>76</v>
       </c>
-      <c r="E28" s="1" t="s">
+      <c r="I32" s="25" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+    <row r="33" spans="1:9" s="39" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="24" t="s">
+        <v>73</v>
+      </c>
+      <c r="B33" s="39" t="s">
+        <v>112</v>
+      </c>
+      <c r="C33" s="39" t="s">
+        <v>21</v>
+      </c>
+      <c r="D33" s="39" t="s">
+        <v>19</v>
+      </c>
+      <c r="E33" s="39">
+        <v>1</v>
+      </c>
+      <c r="F33" s="39">
+        <v>1</v>
+      </c>
+      <c r="G33" s="39">
+        <v>1</v>
+      </c>
+      <c r="H33" s="40" t="s">
+        <v>110</v>
+      </c>
+      <c r="I33" s="40" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" s="41" customFormat="1" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="B34" s="41" t="s">
+        <v>115</v>
+      </c>
+      <c r="C34" s="41" t="s">
+        <v>21</v>
+      </c>
+      <c r="D34" s="41" t="s">
+        <v>19</v>
+      </c>
+      <c r="E34" s="41">
+        <v>1</v>
+      </c>
+      <c r="F34" s="41">
+        <v>1</v>
+      </c>
+      <c r="G34" s="41">
+        <v>1</v>
+      </c>
+      <c r="H34" s="42" t="s">
+        <v>110</v>
+      </c>
+      <c r="I34" s="42" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" s="6" customFormat="1" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="B29" t="s">
+      <c r="C35" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="C29" t="s">
+      <c r="D35" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="D29" s="1" t="s">
+      <c r="E35" s="6">
+        <v>1</v>
+      </c>
+      <c r="F35" s="6">
+        <v>1</v>
+      </c>
+      <c r="G35" s="6">
+        <v>1</v>
+      </c>
+      <c r="H35" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="E29" s="1" t="s">
+      <c r="I35" s="8" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="30" spans="1:5" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="6" t="s">
+    <row r="36" spans="1:9" s="5" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="B30" s="6" t="s">
+      <c r="C36" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="C30" s="6" t="s">
+      <c r="D36" s="5" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="6" t="s">
+      <c r="E36" s="5">
+        <v>1</v>
+      </c>
+      <c r="F36" s="5">
+        <v>1</v>
+      </c>
+      <c r="G36" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" s="5" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="H37" s="35" t="s">
+        <v>106</v>
+      </c>
+      <c r="I37" s="35" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" s="5" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="26" t="s">
+        <v>81</v>
+      </c>
+      <c r="H38" s="35" t="s">
+        <v>108</v>
+      </c>
+      <c r="I38" s="35" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" s="5" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="H39" s="35" t="s">
+        <v>105</v>
+      </c>
+      <c r="I39" s="35" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="B31" s="6" t="s">
+      <c r="B40" s="5"/>
+      <c r="C40" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="C31" s="6" t="s">
+      <c r="D40" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E31" s="1" t="s">
+      <c r="E40" s="5">
+        <v>1</v>
+      </c>
+      <c r="F40" s="5"/>
+      <c r="G40" s="5"/>
+      <c r="I40" s="1" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="32" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
+    <row r="41" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="B32" s="3" t="s">
+      <c r="B41" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C41" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C32" s="3" t="s">
+      <c r="D41" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D32" s="4" t="s">
+      <c r="E41" s="3">
+        <v>1</v>
+      </c>
+      <c r="H41" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="E32" s="4" t="s">
+      <c r="I41" s="4" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="33" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="34" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="35" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="36" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="37" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="38" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="39" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="40" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="42" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="43" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="44" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="45" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="46" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="47" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="48" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="49" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1"/>
-    <hyperlink ref="E3" r:id="rId2"/>
-    <hyperlink ref="E4" r:id="rId3"/>
-    <hyperlink ref="E5" r:id="rId4"/>
-    <hyperlink ref="E8" r:id="rId5"/>
-    <hyperlink ref="D8" r:id="rId6"/>
-    <hyperlink ref="D11" r:id="rId7"/>
-    <hyperlink ref="E12" r:id="rId8"/>
-    <hyperlink ref="D13" r:id="rId9"/>
-    <hyperlink ref="D16" r:id="rId10"/>
-    <hyperlink ref="E15" r:id="rId11"/>
-    <hyperlink ref="E20" r:id="rId12"/>
-    <hyperlink ref="D20" r:id="rId13"/>
-    <hyperlink ref="E21" r:id="rId14"/>
-    <hyperlink ref="D19" r:id="rId15"/>
-    <hyperlink ref="E19" r:id="rId16"/>
-    <hyperlink ref="D22" r:id="rId17"/>
-    <hyperlink ref="D23" r:id="rId18"/>
-    <hyperlink ref="E24" r:id="rId19"/>
-    <hyperlink ref="D24" r:id="rId20"/>
-    <hyperlink ref="D25" r:id="rId21"/>
-    <hyperlink ref="D26" r:id="rId22"/>
-    <hyperlink ref="D27" r:id="rId23"/>
-    <hyperlink ref="E28" r:id="rId24"/>
-    <hyperlink ref="D28" r:id="rId25"/>
-    <hyperlink ref="E29" r:id="rId26"/>
-    <hyperlink ref="D29" r:id="rId27"/>
-    <hyperlink ref="E31" r:id="rId28"/>
-    <hyperlink ref="E32" r:id="rId29"/>
-    <hyperlink ref="D32" r:id="rId30"/>
+    <hyperlink ref="I2" r:id="rId1"/>
+    <hyperlink ref="I4" r:id="rId2"/>
+    <hyperlink ref="I5" r:id="rId3"/>
+    <hyperlink ref="I6" r:id="rId4"/>
+    <hyperlink ref="I9" r:id="rId5"/>
+    <hyperlink ref="H9" r:id="rId6"/>
+    <hyperlink ref="H12" r:id="rId7"/>
+    <hyperlink ref="I13" r:id="rId8"/>
+    <hyperlink ref="H15" r:id="rId9"/>
+    <hyperlink ref="H18" r:id="rId10"/>
+    <hyperlink ref="I17" r:id="rId11"/>
+    <hyperlink ref="I24" r:id="rId12"/>
+    <hyperlink ref="H24" r:id="rId13"/>
+    <hyperlink ref="I25" r:id="rId14"/>
+    <hyperlink ref="H23" r:id="rId15"/>
+    <hyperlink ref="I23" r:id="rId16"/>
+    <hyperlink ref="H26" r:id="rId17"/>
+    <hyperlink ref="H27" r:id="rId18"/>
+    <hyperlink ref="I28" r:id="rId19"/>
+    <hyperlink ref="H28" r:id="rId20"/>
+    <hyperlink ref="H29" r:id="rId21"/>
+    <hyperlink ref="H30" r:id="rId22"/>
+    <hyperlink ref="H31" r:id="rId23"/>
+    <hyperlink ref="I32" r:id="rId24"/>
+    <hyperlink ref="H32" r:id="rId25"/>
+    <hyperlink ref="I35" r:id="rId26"/>
+    <hyperlink ref="H35" r:id="rId27"/>
+    <hyperlink ref="I40" r:id="rId28"/>
+    <hyperlink ref="I41" r:id="rId29"/>
+    <hyperlink ref="H41" r:id="rId30"/>
+    <hyperlink ref="I20" r:id="rId31"/>
+    <hyperlink ref="H10" r:id="rId32"/>
+    <hyperlink ref="I11" r:id="rId33"/>
+    <hyperlink ref="H11" r:id="rId34"/>
+    <hyperlink ref="H7" r:id="rId35"/>
+    <hyperlink ref="H17" r:id="rId36"/>
+    <hyperlink ref="H14" r:id="rId37"/>
+    <hyperlink ref="I39" r:id="rId38"/>
+    <hyperlink ref="H39" r:id="rId39"/>
+    <hyperlink ref="H37" r:id="rId40"/>
+    <hyperlink ref="I37" r:id="rId41"/>
+    <hyperlink ref="H38" r:id="rId42"/>
+    <hyperlink ref="I38" r:id="rId43"/>
+    <hyperlink ref="H33" r:id="rId44"/>
+    <hyperlink ref="H3" r:id="rId45"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId31"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId46"/>
 </worksheet>
 </file>
</xml_diff>